<commit_message>
updated Ui on feb 6th
</commit_message>
<xml_diff>
--- a/RestApi/source/summaryDataChanged.xlsx
+++ b/RestApi/source/summaryDataChanged.xlsx
@@ -14,63 +14,180 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
-  <si>
-    <t>LT_SnapshotMemberID</t>
-  </si>
-  <si>
-    <t>TT_RawDataMemberID</t>
-  </si>
-  <si>
-    <t>TT_Raw_Data_MemberID</t>
-  </si>
-  <si>
-    <t>s6OA0T41m85XOrP6Z4yIoBpWmss=</t>
-  </si>
-  <si>
-    <t>gzwOChVd0pN5C5slAhITygulyvc=</t>
-  </si>
-  <si>
-    <t>qKcj23RfwXc5oBUlQqT9J4eibu8=</t>
-  </si>
-  <si>
-    <t>zyoQ5HTom/jpGITCsA8lYEUnQq8=</t>
-  </si>
-  <si>
-    <t>p31f1v/p9qZSUVBsND+hrt5HSbY=</t>
-  </si>
-  <si>
-    <t>HNjHve5VAqI4dSv2jBa6VZfF5uY=</t>
-  </si>
-  <si>
-    <t>3KzgKrf/eBlF6ruCZTUVWFYaFBA=</t>
-  </si>
-  <si>
-    <t>nwW2ZdrRkCO4nU5HQuGiT4aS6nw=</t>
-  </si>
-  <si>
-    <t>jfFJIwyJmIDQXBHIgC/6fL/AGKk=</t>
-  </si>
-  <si>
-    <t>0BPTD4j1DnB/Ak/rClDu0IfMAXs=</t>
-  </si>
-  <si>
-    <t>IU03zfJ0IhI2vyDkWEFvvKWwffs=</t>
-  </si>
-  <si>
-    <t>MyBu4rJgOzYvPnTiQVX5Ae65TwI=</t>
-  </si>
-  <si>
-    <t>BjAxC8E2DSsGpBITtCRbIQD11Sc=</t>
-  </si>
-  <si>
-    <t>mnbUmBAIwQRr8/mbtj8Kd+15sS0=</t>
-  </si>
-  <si>
-    <t>jt9IOi1yWROL5Jel3ynJMdh6i/k=</t>
-  </si>
-  <si>
-    <t>sReep6SaoiEd0ukZONefyOMtNWk=</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="58">
+  <si>
+    <t>LT_Raw_Data</t>
+  </si>
+  <si>
+    <t>LT_Snapshot</t>
+  </si>
+  <si>
+    <t>LT_Snapshot_Not_Matched_Column</t>
+  </si>
+  <si>
+    <t>Standard Studio</t>
+  </si>
+  <si>
+    <t>NI Number, Member Identifier</t>
+  </si>
+  <si>
+    <t>Member Identifier</t>
+  </si>
+  <si>
+    <t>DCPS, DJC</t>
+  </si>
+  <si>
+    <t>Total Pension at Exit</t>
+  </si>
+  <si>
+    <t>Level Pen at DOE (A)</t>
+  </si>
+  <si>
+    <t>Escalating Pension at DOE (A), Escalating Pension at DOE (I)</t>
+  </si>
+  <si>
+    <t>Post 97 Sch Pen subjct LPI at DOE (A), Post 97 Sch Pen subjct LPI at DOE (I)</t>
+  </si>
+  <si>
+    <t>Pst2006 2.5% subj LPI @ DOE (A)</t>
+  </si>
+  <si>
+    <t>Post09 Escalating Pension @ DOE (A)</t>
+  </si>
+  <si>
+    <t>Subdivision code</t>
+  </si>
+  <si>
+    <t>NRA</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Surname</t>
+  </si>
+  <si>
+    <t>DOB</t>
+  </si>
+  <si>
+    <t>DJC</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>NRD</t>
+  </si>
+  <si>
+    <t>Date of Exit</t>
+  </si>
+  <si>
+    <t>Post Code</t>
+  </si>
+  <si>
+    <t>Unique ID</t>
+  </si>
+  <si>
+    <t>EmployeeIDNumber</t>
+  </si>
+  <si>
+    <t>EIDNumber_Received</t>
+  </si>
+  <si>
+    <t>MembershipDate1</t>
+  </si>
+  <si>
+    <t>AccruedBenefit1</t>
+  </si>
+  <si>
+    <t>AccBen1_XSNonRev</t>
+  </si>
+  <si>
+    <t>AccBen1_XSRev</t>
+  </si>
+  <si>
+    <t>AccBen1_Post97PreA</t>
+  </si>
+  <si>
+    <t>AccBen1_PostAPre09</t>
+  </si>
+  <si>
+    <t>AccBen1_Post09</t>
+  </si>
+  <si>
+    <t>BenefitSetShortName</t>
+  </si>
+  <si>
+    <t>OrganizationCode</t>
+  </si>
+  <si>
+    <t>DivisionCode</t>
+  </si>
+  <si>
+    <t>SubDivisionCode</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>BirthDate</t>
+  </si>
+  <si>
+    <t>HireDate1</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>NormalRetAge</t>
+  </si>
+  <si>
+    <t>PayStatus</t>
+  </si>
+  <si>
+    <t>ParticipantStatus</t>
+  </si>
+  <si>
+    <t>USC</t>
+  </si>
+  <si>
+    <t>MembershipDate2</t>
+  </si>
+  <si>
+    <t>HealthStatus</t>
+  </si>
+  <si>
+    <t>AliveStatus</t>
+  </si>
+  <si>
+    <t>TerminationDate1</t>
+  </si>
+  <si>
+    <t>ImportName</t>
+  </si>
+  <si>
+    <t>USC_P</t>
+  </si>
+  <si>
+    <t>PostCode2</t>
+  </si>
+  <si>
+    <t>Franked</t>
+  </si>
+  <si>
+    <t>UnitCode</t>
+  </si>
+  <si>
+    <t>CATCODE</t>
+  </si>
+  <si>
+    <t>UNITIND</t>
+  </si>
+  <si>
+    <t>CategoryCode2</t>
+  </si>
+  <si>
+    <t>CategoryCode3</t>
   </si>
 </sst>
 </file>
@@ -428,7 +545,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -453,10 +570,10 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -467,10 +584,10 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -481,10 +598,10 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -495,10 +612,10 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -508,8 +625,11 @@
       <c r="B6" t="s">
         <v>7</v>
       </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -519,8 +639,264 @@
       <c r="B7" t="s">
         <v>8</v>
       </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
       <c r="D7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
         <v>18</v>
+      </c>
+      <c r="C18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>